<commit_message>
plaatjes insertion and inverse mutation
</commit_message>
<xml_diff>
--- a/pictures/Bob mutatie plaatjes.xlsx
+++ b/pictures/Bob mutatie plaatjes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobbo\Dropbox\Artificial Intelligence\Evolutionary Computing\Project\Team36-EC_project\pictures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\Evolutionary_Computing\Team36-EC_project\pictures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE7067B1-1AEC-4CCE-A34B-3557074CCE23}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE4B64B-085E-4D68-9D8A-8093FC183E5A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{CB099D01-2E9D-4EE6-BAE6-3169E2C79076}"/>
   </bookViews>
@@ -99,7 +99,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -233,6 +233,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -242,14 +246,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -482,7 +482,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -781,7 +781,7 @@
   <dimension ref="B11:Z33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="75" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,95 +802,95 @@
     </row>
     <row r="14" spans="3:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="C15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="9"/>
-      <c r="Q15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="9"/>
+      <c r="C15" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="13"/>
+      <c r="Q15" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="13"/>
     </row>
     <row r="16" spans="3:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="10">
-        <v>0</v>
-      </c>
-      <c r="D16" s="11">
-        <v>1</v>
-      </c>
-      <c r="E16" s="11">
-        <v>2</v>
-      </c>
-      <c r="F16" s="11">
-        <v>3</v>
-      </c>
-      <c r="G16" s="11">
-        <v>4</v>
-      </c>
-      <c r="H16" s="11">
+      <c r="C16" s="7">
+        <v>0</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8">
+        <v>2</v>
+      </c>
+      <c r="F16" s="8">
+        <v>3</v>
+      </c>
+      <c r="G16" s="8">
+        <v>4</v>
+      </c>
+      <c r="H16" s="8">
         <v>5</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="8">
         <v>6</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="8">
         <v>7</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="8">
         <v>8</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="9">
         <v>9</v>
       </c>
-      <c r="Q16" s="10">
-        <v>0</v>
-      </c>
-      <c r="R16" s="11">
-        <v>1</v>
-      </c>
-      <c r="S16" s="11">
-        <v>2</v>
-      </c>
-      <c r="T16" s="11">
-        <v>3</v>
-      </c>
-      <c r="U16" s="11">
-        <v>4</v>
-      </c>
-      <c r="V16" s="11">
+      <c r="Q16" s="7">
+        <v>0</v>
+      </c>
+      <c r="R16" s="8">
+        <v>1</v>
+      </c>
+      <c r="S16" s="8">
+        <v>2</v>
+      </c>
+      <c r="T16" s="8">
+        <v>3</v>
+      </c>
+      <c r="U16" s="8">
+        <v>4</v>
+      </c>
+      <c r="V16" s="8">
         <v>5</v>
       </c>
-      <c r="W16" s="11">
+      <c r="W16" s="8">
         <v>6</v>
       </c>
-      <c r="X16" s="11">
+      <c r="X16" s="8">
         <v>7</v>
       </c>
-      <c r="Y16" s="11">
+      <c r="Y16" s="8">
         <v>8</v>
       </c>
-      <c r="Z16" s="12">
+      <c r="Z16" s="9">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="2">
@@ -926,7 +926,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="13" t="s">
+      <c r="P17" s="10" t="s">
         <v>0</v>
       </c>
       <c r="Q17" s="2">
@@ -967,95 +967,95 @@
     </row>
     <row r="22" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="C23" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="9"/>
-      <c r="Q23" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="8"/>
-      <c r="W23" s="8"/>
-      <c r="X23" s="8"/>
-      <c r="Y23" s="8"/>
-      <c r="Z23" s="9"/>
+      <c r="C23" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="13"/>
+      <c r="Q23" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
+      <c r="Z23" s="13"/>
     </row>
     <row r="24" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="10">
-        <v>0</v>
-      </c>
-      <c r="D24" s="11">
-        <v>1</v>
-      </c>
-      <c r="E24" s="11">
-        <v>2</v>
-      </c>
-      <c r="F24" s="11">
-        <v>3</v>
-      </c>
-      <c r="G24" s="11">
-        <v>4</v>
-      </c>
-      <c r="H24" s="11">
+      <c r="C24" s="7">
+        <v>0</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="E24" s="8">
+        <v>2</v>
+      </c>
+      <c r="F24" s="8">
+        <v>3</v>
+      </c>
+      <c r="G24" s="8">
+        <v>4</v>
+      </c>
+      <c r="H24" s="8">
         <v>5</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I24" s="8">
         <v>6</v>
       </c>
-      <c r="J24" s="11">
+      <c r="J24" s="8">
         <v>7</v>
       </c>
-      <c r="K24" s="11">
+      <c r="K24" s="8">
         <v>8</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L24" s="9">
         <v>9</v>
       </c>
-      <c r="Q24" s="10">
-        <v>0</v>
-      </c>
-      <c r="R24" s="11">
-        <v>1</v>
-      </c>
-      <c r="S24" s="11">
-        <v>2</v>
-      </c>
-      <c r="T24" s="11">
-        <v>3</v>
-      </c>
-      <c r="U24" s="11">
-        <v>4</v>
-      </c>
-      <c r="V24" s="11">
+      <c r="Q24" s="7">
+        <v>0</v>
+      </c>
+      <c r="R24" s="8">
+        <v>1</v>
+      </c>
+      <c r="S24" s="8">
+        <v>2</v>
+      </c>
+      <c r="T24" s="8">
+        <v>3</v>
+      </c>
+      <c r="U24" s="8">
+        <v>4</v>
+      </c>
+      <c r="V24" s="8">
         <v>5</v>
       </c>
-      <c r="W24" s="11">
+      <c r="W24" s="8">
         <v>6</v>
       </c>
-      <c r="X24" s="11">
+      <c r="X24" s="8">
         <v>7</v>
       </c>
-      <c r="Y24" s="11">
+      <c r="Y24" s="8">
         <v>8</v>
       </c>
-      <c r="Z24" s="12">
+      <c r="Z24" s="9">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="2">
@@ -1091,7 +1091,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="13" t="s">
+      <c r="P25" s="10" t="s">
         <v>0</v>
       </c>
       <c r="Q25" s="2">
@@ -1127,95 +1127,95 @@
     </row>
     <row r="29" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="C30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="9"/>
-      <c r="Q30" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
-      <c r="Y30" s="8"/>
-      <c r="Z30" s="9"/>
+      <c r="C30" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="13"/>
+      <c r="Q30" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="13"/>
     </row>
     <row r="31" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="10">
-        <v>0</v>
-      </c>
-      <c r="D31" s="11">
-        <v>1</v>
-      </c>
-      <c r="E31" s="11">
-        <v>2</v>
-      </c>
-      <c r="F31" s="11">
-        <v>3</v>
-      </c>
-      <c r="G31" s="11">
-        <v>4</v>
-      </c>
-      <c r="H31" s="11">
+      <c r="C31" s="7">
+        <v>0</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+      <c r="E31" s="8">
+        <v>2</v>
+      </c>
+      <c r="F31" s="8">
+        <v>3</v>
+      </c>
+      <c r="G31" s="8">
+        <v>4</v>
+      </c>
+      <c r="H31" s="8">
         <v>5</v>
       </c>
-      <c r="I31" s="11">
+      <c r="I31" s="8">
         <v>6</v>
       </c>
-      <c r="J31" s="11">
+      <c r="J31" s="8">
         <v>7</v>
       </c>
-      <c r="K31" s="11">
+      <c r="K31" s="8">
         <v>8</v>
       </c>
-      <c r="L31" s="12">
+      <c r="L31" s="9">
         <v>9</v>
       </c>
-      <c r="Q31" s="10">
-        <v>0</v>
-      </c>
-      <c r="R31" s="11">
-        <v>1</v>
-      </c>
-      <c r="S31" s="11">
-        <v>2</v>
-      </c>
-      <c r="T31" s="11">
-        <v>3</v>
-      </c>
-      <c r="U31" s="11">
-        <v>4</v>
-      </c>
-      <c r="V31" s="11">
+      <c r="Q31" s="7">
+        <v>0</v>
+      </c>
+      <c r="R31" s="8">
+        <v>1</v>
+      </c>
+      <c r="S31" s="8">
+        <v>2</v>
+      </c>
+      <c r="T31" s="8">
+        <v>3</v>
+      </c>
+      <c r="U31" s="8">
+        <v>4</v>
+      </c>
+      <c r="V31" s="8">
         <v>5</v>
       </c>
-      <c r="W31" s="11">
+      <c r="W31" s="8">
         <v>6</v>
       </c>
-      <c r="X31" s="11">
+      <c r="X31" s="8">
         <v>7</v>
       </c>
-      <c r="Y31" s="11">
+      <c r="Y31" s="8">
         <v>8</v>
       </c>
-      <c r="Z31" s="12">
+      <c r="Z31" s="9">
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="2">
@@ -1251,7 +1251,7 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="13" t="s">
+      <c r="P32" s="10" t="s">
         <v>4</v>
       </c>
       <c r="Q32" s="2">
@@ -1286,7 +1286,7 @@
       </c>
     </row>
     <row r="33" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="2">
@@ -1322,7 +1322,7 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="13" t="s">
+      <c r="P33" s="10" t="s">
         <v>5</v>
       </c>
       <c r="Q33" s="2">

</xml_diff>